<commit_message>
bug fixed and updated mapping logic of death
1. debug: drug_type_id = 32818 for vaccination
2. Update: withinTheObservationPeriod flag is effective to Death under the condition: accept Death outside the observation period only if after max threshold and within 3 months
</commit_message>
<xml_diff>
--- a/reference/Covid-19 vaccine mapping.xlsx
+++ b/reference/Covid-19 vaccine mapping.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\ETL-CDMBuilder\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD61F8C6-84BE-49F7-87F1-BD66E881D7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFED5E5F-C936-4AF8-B643-70DC2B22D5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{21B7E9B4-A9E6-41AC-9EF3-DA2BC3B8A79B}"/>
+    <workbookView xWindow="4215" yWindow="3390" windowWidth="25125" windowHeight="11295" activeTab="3" xr2:uid="{21B7E9B4-A9E6-41AC-9EF3-DA2BC3B8A79B}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping suggest for gold 202207" sheetId="1" r:id="rId1"/>
     <sheet name="read code" sheetId="2" r:id="rId2"/>
     <sheet name="COVID Vaccine Brand Feb 22" sheetId="3" r:id="rId3"/>
+    <sheet name="mapping suggest for gold 202301" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'mapping suggest for gold 202207'!$A$2:$H$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="103">
   <si>
     <t>COVOXFORD</t>
   </si>
@@ -111,9 +112,6 @@
   </si>
   <si>
     <t>COVOTHER</t>
-  </si>
-  <si>
-    <t>COVCOURAGEOUS</t>
   </si>
   <si>
     <t>COVTALENT</t>
@@ -278,9 +276,6 @@
     <t>COVID-19 Vaccine Covaxin (NIV-2020-770 inactivated) 6micrograms/0.5ml dose suspension for injection vials (Bharat Biotech International Ltd)</t>
   </si>
   <si>
-    <t>COVID-19 Vaccine Covaxin (NIV-2020-770 inactivated) 6micrograms/0.5ml dose suspension for injection multidose vials (Bharat Biotech International Ltd)</t>
-  </si>
-  <si>
     <t>concept_class_id</t>
   </si>
   <si>
@@ -309,13 +304,118 @@
   </si>
   <si>
     <t>SARS-COV-2 (COVID-19) vaccine, vector non-replicating, recombinant spike protein-Ad26, preservative free, 0.5 mL</t>
+  </si>
+  <si>
+    <t>covid 19 vaccination from immunisation only has immstype, immunisation records can also come from clinical</t>
+  </si>
+  <si>
+    <t>Immunisation course to maintain protection against SARS-CoV-2 (severe acute respiratory syndrome coronavirus 2)</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <r>
+      <t>Medical History Entry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> of '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>65F0800</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> Immunisation course to maintain protection against SARS-CoV-2': -&gt; Procedure -&gt; no effect</t>
+    </r>
+  </si>
+  <si>
+    <t>Generic COVID-19 Vaccine Novavax (adjuvanted) 5micrograms/0.5ml dose suspension for injection multidose vials</t>
+  </si>
+  <si>
+    <t>Talent 0.5ml dose solution for injection multidose vials (Secretary of State for Health)</t>
+  </si>
+  <si>
+    <t>Generic COVID-19 Vaccine AstraZeneca (ChAdOx1 S [recombinant]) 5x10,000,000,000 viral particles/0.5ml dose solution for injection multidose vials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productname </t>
+  </si>
+  <si>
+    <t>RxNorm Extension</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccine, recombinant, full-length nanoparticle spike (S) protein, adjuvanted with Matrix-M Injectable Suspension</t>
+  </si>
+  <si>
+    <t>Clinical Drug Form</t>
+  </si>
+  <si>
+    <t>Drug</t>
+  </si>
+  <si>
+    <t>00780022</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccine, recombinant, plant-derived Virus-Like Particle (VLP) spike (S) protein, adjuvanted with AS03 Injectable Suspension</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 Inactivated Virus Non-US Vaccine Product (COVAXIN)</t>
+  </si>
+  <si>
+    <t>concept_id</t>
+  </si>
+  <si>
+    <t>domain_id</t>
+  </si>
+  <si>
+    <t>vocabulary_id</t>
+  </si>
+  <si>
+    <t>standard_concept</t>
+  </si>
+  <si>
+    <t>concept_code</t>
+  </si>
+  <si>
+    <t>valid_start_date</t>
+  </si>
+  <si>
+    <t>valid_end_date</t>
+  </si>
+  <si>
+    <t>invalid_reason</t>
+  </si>
+  <si>
+    <t>Haemophilus influenzae type b, capsular polysaccharide inactivated tetanus toxoid conjugate vaccine</t>
+  </si>
+  <si>
+    <t>Ingredient</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,15 +445,33 @@
       <family val="2"/>
     </font>
     <font>
-      <strike/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +508,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -553,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -592,9 +716,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,6 +730,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,14 +756,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2829823</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>86668</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>105718</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -657,7 +786,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3009900"/>
+          <a:off x="0" y="3028950"/>
           <a:ext cx="15802873" cy="6030268"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -671,13 +800,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>97453</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2314575</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>143824</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1011,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539DD493-5A87-4EF1-9C4E-4C5365340E4D}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A1:XFD11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,31 +1165,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="A1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
+      <c r="K1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1075,7 +1204,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
@@ -1084,25 +1213,25 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="19" t="s">
-        <v>69</v>
+      <c r="N2" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1134,7 +1263,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>2</v>
@@ -1149,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1178,25 +1307,25 @@
         <v>13</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="L4" s="20">
+        <v>74</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="19">
         <v>724907</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="19" t="s">
         <v>3</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1225,25 +1354,25 @@
         <v>13</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="L5" s="20">
+        <v>74</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="19">
         <v>724906</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="19" t="s">
         <v>3</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1272,25 +1401,25 @@
         <v>13</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="L6" s="20">
+      <c r="L6" s="19">
         <v>702866</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1304,7 +1433,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="4">
         <v>724904</v>
@@ -1316,10 +1445,10 @@
         <v>3</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L7" s="4">
         <v>724904</v>
@@ -1331,12 +1460,12 @@
         <v>3</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>23</v>
@@ -1357,10 +1486,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -1378,10 +1507,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -1397,30 +1526,30 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
-        <v>145</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-    </row>
-    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K57" t="s">
-        <v>35</v>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>608585</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1438,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B732161-45B0-4117-B2DC-64A2441A788C}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,55 +1581,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>39</v>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1511,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A59E89-4507-4C29-8A72-800892BAAA60}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,404 +1653,568 @@
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="82.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="64.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="12" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="15" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A7110F-06F4-4BBF-BDE5-082CEA2BAB74}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="141.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="122.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>132</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20">
+        <v>83136</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="27">
+        <v>95962021</v>
+      </c>
+      <c r="F3" s="4">
+        <v>724905</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>133</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3">
+        <v>83125</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="27">
+        <v>95574021</v>
+      </c>
+      <c r="F4" s="4">
+        <v>37003436</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>135</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>83987</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="27">
+        <v>96969021</v>
+      </c>
+      <c r="F5" s="4">
+        <v>37003518</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>134</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>85364</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="27">
+        <v>96497021</v>
+      </c>
+      <c r="F6" s="4">
+        <v>739906</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>143</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>85973</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="4">
+        <v>702666</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>145</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="20">
+        <v>84072</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="27">
+        <v>97549021</v>
+      </c>
+      <c r="F8" s="4">
+        <v>36119721</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>127</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="4">
+        <v>724904</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>130</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="17">
+        <v>83126</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="27">
+        <v>95963021</v>
+      </c>
+      <c r="F10" s="4">
+        <v>724905</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>135</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="3">
+        <v>85827</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>132</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>83126</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="3">
-        <v>95963021</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="4">
-        <v>724905</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>133</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3">
-        <v>83125</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="3">
-        <v>95574021</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="4">
-        <v>37003436</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>135</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3">
-        <v>83987</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="3">
-        <v>96969021</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="4">
-        <v>37003518</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>134</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="3">
-        <v>85364</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="3">
-        <v>96497021</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="4">
-        <v>739906</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>143</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>145</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>127</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="4">
-        <v>724904</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>128</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>130</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="3">
-        <v>85827</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3">
-        <v>85973</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3">
-        <v>86130</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="E11" s="27">
+        <v>99114021</v>
+      </c>
+      <c r="F11" s="4">
+        <v>36119722</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0AB9B4-5192-4BE9-8E4B-80F35935DB89}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>529118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2">
+        <v>798279</v>
+      </c>
+      <c r="H2" s="22">
+        <v>39628</v>
+      </c>
+      <c r="I2" s="22">
+        <v>73050</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>